<commit_message>
update salt prices and loadings in all scenarios
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_corn_HP-salt_10L.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_corn_HP-salt_10L.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\HP_salt_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3D49B6-055F-493E-8B9D-360CE44E6281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0FB3A3-EEF9-44B8-A3B4-AC4B33B48B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -686,7 +686,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A8" sqref="A8:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -972,26 +972,24 @@
         <v>10</v>
       </c>
       <c r="E8" s="3">
-        <v>0.01</v>
+        <v>0.38</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G8" s="3">
-        <f>E8*0.08</f>
-        <v>8.0000000000000004E-4</v>
+        <v>0.34899999999999998</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3">
-        <f>E8*1.2</f>
-        <v>1.2E-2</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
         <v>85</v>
       </c>
       <c r="Q8">
-        <f t="shared" ref="Q8" si="1">IF(E8=H8, 1, IF(F8=$F$2, 1, 0))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1009,19 +1007,17 @@
         <v>10</v>
       </c>
       <c r="E9" s="3">
-        <v>0.01</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="3">
-        <f>E9*0.08</f>
-        <v>8.0000000000000004E-4</v>
+        <v>0.65700000000000003</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3">
-        <f>E9*1.2</f>
-        <v>1.2E-2</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
@@ -1323,7 +1319,7 @@
         <v>79</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" ref="Q17:Q18" si="2">IF(E17=H17, 1, IF(F17=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q17:Q18" si="1">IF(E17=H17, 1, IF(F17=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1360,7 +1356,7 @@
         <v>78</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -1436,7 +1432,7 @@
         <v>64</v>
       </c>
       <c r="Q20">
-        <f t="shared" ref="Q20" si="3">IF(E20=H20, 1, IF(F20=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q20" si="2">IF(E20=H20, 1, IF(F20=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1729,7 +1725,7 @@
         <v>65</v>
       </c>
       <c r="Q28">
-        <f t="shared" ref="Q28" si="4">IF(E28=H28, 1, IF(F28=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q28" si="3">IF(E28=H28, 1, IF(F28=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1766,7 +1762,7 @@
         <v>54</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q29:Q31" si="5">IF(E29=H29, 1, IF(F29=$F$2, 1, 0))</f>
+        <f t="shared" ref="Q29:Q31" si="4">IF(E29=H29, 1, IF(F29=$F$2, 1, 0))</f>
         <v>1</v>
       </c>
     </row>
@@ -1803,7 +1799,7 @@
         <v>38</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>
@@ -1840,7 +1836,7 @@
         <v>50</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update parameter_distributions column name from 'Load Statements' to 'Load statement'
</commit_message>
<xml_diff>
--- a/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_corn_HP-salt_10L.xlsx
+++ b/biorefineries/HP/analyses/full/parameter_distributions/HP_salt_product/parameter-distributions_corn_HP-salt_10L.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saran\Documents\Academia\repository_clones\Bioindustrial-Park\biorefineries\HP\analyses\full\parameter_distributions\HP_salt_product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0FB3A3-EEF9-44B8-A3B4-AC4B33B48B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DBAB9C-1EBB-4F3A-98E6-8F4A22A98851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>Baseline</t>
   </si>
   <si>
-    <t>Load Statements</t>
-  </si>
-  <si>
     <t>g/L/h</t>
   </si>
   <si>
@@ -315,6 +312,9 @@
   </si>
   <si>
     <t>Product HP salt storage time</t>
+  </si>
+  <si>
+    <t>Load statement</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,10 +728,10 @@
         <v>6</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>29</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">
@@ -762,7 +762,7 @@
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2">
         <f>IF(E2=H2, 1, IF(F2=$F$2, 1, 0))</f>
@@ -771,7 +771,7 @@
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -780,13 +780,13 @@
         <v>26</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="4">
         <v>330</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="4">
         <f>0.9*E3</f>
@@ -802,7 +802,7 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="5">
         <f>IF(E3=H3, 1, IF(F3=$F$2, 1, 0))</f>
@@ -826,7 +826,7 @@
         <v>0.13900000000000001</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G4" s="4">
         <v>0.127</v>
@@ -840,7 +840,7 @@
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q4" s="5">
         <f t="shared" ref="Q4:Q27" si="0">IF(E4=H4, 1, IF(F4=$F$2, 1, 0))</f>
@@ -864,7 +864,7 @@
         <v>0.27650000000000002</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G5" s="3">
         <v>0.21629999999999999</v>
@@ -877,7 +877,7 @@
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
@@ -901,7 +901,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3">
         <v>6.7000000000000004E-2</v>
@@ -914,7 +914,7 @@
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
@@ -923,7 +923,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
@@ -951,7 +951,7 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -960,7 +960,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>7</v>
@@ -986,7 +986,7 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
@@ -995,7 +995,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>7</v>
@@ -1045,7 +1045,7 @@
         <v>0.28599999999999998</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3">
         <v>0.17499999999999999</v>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>7</v>
@@ -1082,7 +1082,7 @@
         <v>0.10355</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" s="3">
         <f>E11*0.9</f>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
@@ -1106,7 +1106,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>7</v>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>7</v>
@@ -1150,13 +1150,13 @@
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="3">
         <v>134000</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13">
         <f>E13*0.8</f>
@@ -1172,7 +1172,7 @@
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
@@ -1181,7 +1181,7 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
@@ -1207,7 +1207,7 @@
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
@@ -1216,7 +1216,7 @@
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>7</v>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q15">
         <f t="shared" si="0"/>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>27</v>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="J16" s="7"/>
       <c r="K16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q16">
         <f t="shared" si="0"/>
@@ -1288,10 +1288,10 @@
     </row>
     <row r="17" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>27</v>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="J17" s="4"/>
       <c r="K17" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q17" s="5">
         <f t="shared" ref="Q17:Q18" si="1">IF(E17=H17, 1, IF(F17=$F$2, 1, 0))</f>
@@ -1325,10 +1325,10 @@
     </row>
     <row r="18" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>27</v>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q18" s="5">
         <f t="shared" si="1"/>
@@ -1362,23 +1362,23 @@
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="4">
         <f>0.423/2</f>
         <v>0.21149999999999999</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G19" s="4">
         <f>E19*0.8</f>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q19" s="5">
         <f t="shared" si="0"/>
@@ -1403,16 +1403,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E20" s="3">
         <v>2</v>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q20">
         <f t="shared" ref="Q20" si="2">IF(E20=H20, 1, IF(F20=$F$2, 1, 0))</f>
@@ -1438,16 +1438,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E21" s="3">
         <v>2</v>
@@ -1464,7 +1464,7 @@
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
@@ -1476,13 +1476,13 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E22" s="3">
         <v>0.95</v>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q22">
         <f t="shared" si="0"/>
@@ -1509,16 +1509,16 @@
     </row>
     <row r="23" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E23" s="4">
         <v>0.05</v>
@@ -1537,7 +1537,7 @@
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q23" s="5">
         <f t="shared" si="0"/>
@@ -1546,10 +1546,10 @@
     </row>
     <row r="24" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>27</v>
@@ -1574,7 +1574,7 @@
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q24" s="5">
         <f t="shared" si="0"/>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="25" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>27</v>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q25" s="5">
         <f t="shared" si="0"/>
@@ -1620,16 +1620,16 @@
     </row>
     <row r="26" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="6">
         <v>0.39</v>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q26" s="5">
         <f t="shared" si="0"/>
@@ -1657,10 +1657,10 @@
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>27</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q27" s="5">
         <f t="shared" si="0"/>
@@ -1694,10 +1694,10 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>27</v>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q28">
         <f t="shared" ref="Q28" si="3">IF(E28=H28, 1, IF(F28=$F$2, 1, 0))</f>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
@@ -1746,7 +1746,7 @@
         <v>168</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G29" s="3">
         <v>134.4</v>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q29">
         <f t="shared" ref="Q29:Q31" si="4">IF(E29=H29, 1, IF(F29=$F$2, 1, 0))</f>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q30">
         <f t="shared" si="4"/>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>23</v>
@@ -1833,7 +1833,7 @@
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q31">
         <f t="shared" si="4"/>

</xml_diff>